<commit_message>
Przed złożeniem wersji testowej
Baza zostanie zreplikowana do wersji DEV. Stworzenie alternatywnego połączenia w oparciu o wersję testową bazy.
</commit_message>
<xml_diff>
--- a/Doc/Samples/Import danych/Medicover/Wzorce/PakietyMediCoverDoPracowników.xlsx
+++ b/Doc/Samples/Import danych/Medicover/Wzorce/PakietyMediCoverDoPracowników.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="9840" windowWidth="28830" windowHeight="3315"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>NazwPracownik</t>
   </si>
@@ -45,7 +45,10 @@
     <t>PrzyczynaOdpisania</t>
   </si>
   <si>
-    <t>c</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ImiePracownik</t>
   </si>
 </sst>
 </file>
@@ -91,9 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -395,55 +399,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <sheetPr codeName="Arkusz1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="1" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -455,6 +463,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Arkusz2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -467,6 +476,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Arkusz3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>